<commit_message>
New game with updated schema
</commit_message>
<xml_diff>
--- a/template_database.xlsx
+++ b/template_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\fifa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AB979D-17CA-42BB-91C9-0CE528168AB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975ED041-78EE-4A6B-AD6B-90AE934DE664}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CF7A23C3-568E-4471-A641-704AE710295D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="6" xr2:uid="{CF7A23C3-568E-4471-A641-704AE710295D}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="172">
   <si>
     <t>user</t>
   </si>
@@ -147,7 +147,7 @@
     <t>Vancouver Whitecaps FC</t>
   </si>
   <si>
-    <t>player</t>
+    <t>competition</t>
   </si>
   <si>
     <t>MLS</t>
@@ -156,6 +156,9 @@
     <t>U.S. Open Cup</t>
   </si>
   <si>
+    <t>division</t>
+  </si>
+  <si>
     <t>Eastern Conference</t>
   </si>
   <si>
@@ -492,9 +495,6 @@
     <t>teamId</t>
   </si>
   <si>
-    <t>competitionId</t>
-  </si>
-  <si>
     <t>birthDate</t>
   </si>
   <si>
@@ -541,9 +541,6 @@
   </si>
   <si>
     <t>fixtureId</t>
-  </si>
-  <si>
-    <t>gameId</t>
   </si>
   <si>
     <t>FIFA 20</t>
@@ -970,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7C6B2E-3A25-4793-B219-EF35B0E4841D}">
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,7 +982,7 @@
     <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.88671875" bestFit="1" customWidth="1"/>
@@ -1014,7 +1011,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1026,7 +1023,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -1040,10 +1037,13 @@
       <c r="I2" t="s">
         <v>7</v>
       </c>
+      <c r="J2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>161</v>
@@ -1073,22 +1073,16 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -1096,16 +1090,16 @@
         <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>151</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
@@ -1119,72 +1113,72 @@
         <v>155</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
         <v>152</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="P8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="T8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="U8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="V8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="W8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
         <v>157</v>
@@ -1193,7 +1187,7 @@
         <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1204,7 +1198,7 @@
         <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -1218,13 +1212,13 @@
         <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D11" t="s">
         <v>155</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
@@ -1252,7 +1246,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
         <v>157</v>
@@ -1261,7 +1255,7 @@
         <v>155</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
         <v>166</v>
@@ -1292,167 +1286,167 @@
         <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
         <v>155</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1472,7 +1466,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1485,12 +1479,12 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:H1"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
@@ -1560,7 +1554,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A24"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,7 +1570,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="9"/>
       <c r="E2" s="3"/>
@@ -1586,7 +1580,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" s="9"/>
       <c r="E3" s="3"/>
@@ -1828,7 +1822,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1862,7 +1856,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1877,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>161</v>
@@ -1885,7 +1879,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -1923,863 +1917,676 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85211A1D-C55C-4B45-9CDA-9B78EAA02CD1}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>157</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="9" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" t="str">
-        <f>_xlfn.CONCAT("false")</f>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E47" si="0">_xlfn.CONCAT("false")</f>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>168</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" t="s">
+        <v>167</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>167</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>168</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="9" t="s">
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="9" t="s">
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>168</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>167</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>168</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" t="s">
-        <v>168</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="9" t="s">
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>168</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="9" t="s">
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" t="s">
-        <v>168</v>
-      </c>
-      <c r="E22" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>168</v>
-      </c>
-      <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="9" t="s">
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
+        <v>167</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
-        <v>168</v>
-      </c>
-      <c r="E24" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" t="s">
-        <v>168</v>
-      </c>
-      <c r="E25" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" t="s">
-        <v>168</v>
-      </c>
-      <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" t="s">
-        <v>168</v>
-      </c>
-      <c r="E27" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" t="s">
-        <v>168</v>
-      </c>
-      <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" t="s">
-        <v>168</v>
-      </c>
-      <c r="E29" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" t="s">
-        <v>168</v>
-      </c>
-      <c r="E30" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" t="s">
-        <v>168</v>
-      </c>
-      <c r="E31" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" t="s">
-        <v>168</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" t="s">
-        <v>168</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" t="s">
-        <v>168</v>
-      </c>
-      <c r="E37" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" t="s">
-        <v>168</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" t="s">
-        <v>168</v>
-      </c>
-      <c r="E39" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" t="s">
-        <v>168</v>
-      </c>
-      <c r="E40" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" t="s">
-        <v>168</v>
-      </c>
-      <c r="E41" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" t="s">
-        <v>168</v>
-      </c>
-      <c r="E42" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" t="s">
-        <v>168</v>
-      </c>
-      <c r="E43" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" t="s">
-        <v>168</v>
-      </c>
-      <c r="E44" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" t="s">
-        <v>168</v>
-      </c>
-      <c r="E45" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" t="s">
-        <v>168</v>
-      </c>
-      <c r="E46" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>34</v>
+      <c r="B47" t="s">
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
-        <v>168</v>
-      </c>
-      <c r="E47" t="str">
-        <f t="shared" si="0"/>
-        <v>false</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2791,7 +2598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECB996B-4EDB-45FF-920C-EBACED915522}">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -2823,114 +2630,114 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
         <v>151</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
         <v>152</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="S1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="T1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="U1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="X1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Y1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Z1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AA1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
       <c r="E2">
         <v>76</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G2" s="11">
         <v>2500</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I2" s="11">
         <v>1000000</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L2" s="11">
         <v>1</v>
@@ -2983,37 +2790,37 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3">
         <v>66</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G3" s="11">
         <v>2500</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I3" s="11">
         <v>1000000</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L3" s="11">
         <v>0</v>
@@ -3066,37 +2873,37 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" s="11">
         <v>70</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G4" s="11">
         <v>2500</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I4" s="11">
         <v>1000000</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L4" s="11">
         <v>0</v>
@@ -3149,37 +2956,37 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>68</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G5" s="11">
         <v>2500</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I5" s="11">
         <v>1000000</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L5" s="11">
         <v>0</v>
@@ -3232,37 +3039,37 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E6" s="11">
         <v>70</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G6" s="11">
         <v>2500</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I6" s="11">
         <v>1000000</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L6" s="11">
         <v>0</v>
@@ -3315,37 +3122,37 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E7" s="11">
         <v>74</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G7" s="11">
         <v>2500</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I7" s="11">
         <v>1000000</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L7" s="11">
         <v>0</v>
@@ -3398,37 +3205,37 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E8" s="11">
         <v>74</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G8" s="11">
         <v>2500</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I8" s="11">
         <v>1000000</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L8" s="11">
         <v>0</v>
@@ -3481,37 +3288,37 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" s="11">
         <v>73</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G9" s="11">
         <v>2500</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I9" s="11">
         <v>1000000</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L9" s="11">
         <v>0</v>
@@ -3564,37 +3371,37 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10">
         <v>75</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G10" s="11">
         <v>2500</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I10" s="11">
         <v>1000000</v>
       </c>
       <c r="J10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L10" s="11">
         <v>0</v>
@@ -3647,37 +3454,37 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="11">
         <v>70</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G11" s="11">
         <v>2500</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I11" s="11">
         <v>1000000</v>
       </c>
       <c r="J11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L11" s="11">
         <v>0</v>
@@ -3730,37 +3537,37 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E12">
         <v>68</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G12" s="11">
         <v>2500</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I12" s="11">
         <v>1000000</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L12" s="11">
         <v>0</v>
@@ -3813,37 +3620,37 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E13" s="11">
         <v>72</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G13" s="11">
         <v>2500</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I13" s="11">
         <v>1000000</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L13" s="11">
         <v>0</v>
@@ -3896,37 +3703,37 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E14">
         <v>69</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G14" s="11">
         <v>2500</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I14" s="11">
         <v>1000000</v>
       </c>
       <c r="J14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L14" s="11">
         <v>0</v>
@@ -3979,37 +3786,37 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E15">
         <v>69</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G15" s="11">
         <v>2500</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I15" s="11">
         <v>1000000</v>
       </c>
       <c r="J15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L15" s="11">
         <v>0</v>
@@ -4062,37 +3869,37 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E16">
         <v>69</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G16" s="11">
         <v>2500</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I16" s="11">
         <v>1000000</v>
       </c>
       <c r="J16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L16" s="11">
         <v>0</v>
@@ -4145,34 +3952,34 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E17">
         <v>68</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G17" s="11">
         <v>2500</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I17" s="11">
         <v>1000000</v>
       </c>
       <c r="J17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L17" s="11">
         <v>0</v>
@@ -4225,37 +4032,37 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E18">
         <v>65</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G18" s="11">
         <v>2500</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I18" s="11">
         <v>1000000</v>
       </c>
       <c r="J18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L18" s="11">
         <v>0</v>
@@ -4308,37 +4115,37 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E19">
         <v>65</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G19" s="11">
         <v>2500</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I19" s="11">
         <v>1000000</v>
       </c>
       <c r="J19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L19" s="11">
         <v>0</v>
@@ -4420,7 +4227,7 @@
         <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4428,13 +4235,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create new copy of competitions
</commit_message>
<xml_diff>
--- a/template_database.xlsx
+++ b/template_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\fifa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975ED041-78EE-4A6B-AD6B-90AE934DE664}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A270404E-AA43-46C7-A9CC-2C11D128DD78}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="6" xr2:uid="{CF7A23C3-568E-4471-A641-704AE710295D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="6" xr2:uid="{CF7A23C3-568E-4471-A641-704AE710295D}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="178">
   <si>
     <t>user</t>
   </si>
@@ -556,6 +556,24 @@
   </si>
   <si>
     <t>FIFA20MLS</t>
+  </si>
+  <si>
+    <t>league</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>2018-01-01T00:00:00.000Z</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>player</t>
   </si>
 </sst>
 </file>
@@ -967,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7C6B2E-3A25-4793-B219-EF35B0E4841D}">
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G6" sqref="B6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,6 +1026,9 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1056,6 +1077,12 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1076,13 +1103,22 @@
         <v>149</v>
       </c>
       <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -1456,17 +1492,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDE56E3-A437-4E4D-9342-95C94441C270}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2">
+        <v>2019</v>
       </c>
     </row>
   </sheetData>
@@ -1479,7 +1526,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1819,31 +1866,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92C7A02-C959-4CBA-A101-0D0CA162AA8F}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="str">
+        <f>_xlfn.CONCAT("true")</f>
+        <v>true</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
+      </c>
+      <c r="B3" t="str">
+        <f>_xlfn.CONCAT("false")</f>
+        <v>false</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1856,7 +1924,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,676 +1985,818 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85211A1D-C55C-4B45-9CDA-9B78EAA02CD1}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D47"/>
+      <selection activeCell="C8" sqref="A1:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
-        <v>167</v>
-      </c>
       <c r="D2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="B3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
-        <v>167</v>
-      </c>
       <c r="D3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
-        <v>167</v>
-      </c>
       <c r="D4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
-        <v>167</v>
-      </c>
       <c r="D5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
-        <v>167</v>
-      </c>
       <c r="D6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
-        <v>167</v>
-      </c>
       <c r="D7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
-        <v>167</v>
-      </c>
       <c r="D8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>167</v>
-      </c>
       <c r="D9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
-        <v>167</v>
-      </c>
       <c r="D10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
-        <v>167</v>
-      </c>
       <c r="D11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>167</v>
-      </c>
       <c r="D12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
-        <v>167</v>
-      </c>
       <c r="D13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
-        <v>167</v>
-      </c>
       <c r="D14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
-        <v>167</v>
-      </c>
       <c r="D15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
-        <v>167</v>
-      </c>
       <c r="D16" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="C17" t="s">
-        <v>167</v>
-      </c>
       <c r="D17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+      <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="s">
-        <v>167</v>
-      </c>
       <c r="D18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
-        <v>167</v>
-      </c>
       <c r="D19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
-        <v>167</v>
-      </c>
       <c r="D20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
-        <v>167</v>
-      </c>
       <c r="D21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
-        <v>167</v>
-      </c>
       <c r="D22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E22">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
+      <c r="B23" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
-        <v>167</v>
-      </c>
       <c r="D23" t="s">
+        <v>167</v>
+      </c>
+      <c r="E23">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
-        <v>167</v>
-      </c>
       <c r="D24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E25">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
       <c r="C28" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
       <c r="C29" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E29">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B30" t="s">
-        <v>37</v>
-      </c>
       <c r="C30" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B31" t="s">
-        <v>37</v>
-      </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B32" t="s">
-        <v>37</v>
-      </c>
       <c r="C32" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
       <c r="C33" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
       <c r="C34" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
       <c r="C35" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E35">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
       <c r="C36" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
       <c r="C37" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B38" t="s">
-        <v>37</v>
-      </c>
       <c r="C38" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
       <c r="C39" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
       <c r="C40" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B41" t="s">
-        <v>37</v>
-      </c>
       <c r="C41" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E41">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B42" t="s">
-        <v>37</v>
-      </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E42">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
       <c r="C43" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B44" t="s">
-        <v>37</v>
-      </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B45" t="s">
-        <v>37</v>
-      </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B46" t="s">
-        <v>37</v>
-      </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B47" t="s">
-        <v>37</v>
-      </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>37</v>
+        <v>167</v>
+      </c>
+      <c r="E47">
+        <v>2019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>